<commit_message>
add revised figures to text and suppmat
</commit_message>
<xml_diff>
--- a/tables/table2.xlsx
+++ b/tables/table2.xlsx
@@ -24,17 +24,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
-  <si>
-    <t>Bootstrap-simulation evaluations</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Uncertainty scenarios</t>
   </si>
   <si>
-    <t>Description</t>
-  </si>
-  <si>
     <t>Base</t>
   </si>
   <si>
@@ -59,38 +53,44 @@
     <t>Aggregation treatment</t>
   </si>
   <si>
-    <t>Standard bootstrap-simulation ommiting steps 5 and 6 that include ageing error and growth variability</t>
-  </si>
-  <si>
     <t>Bootstrap-simulation including ageing error only</t>
   </si>
   <si>
     <t>Bootstrap-simulation including growth variabliity only</t>
   </si>
   <si>
-    <t>Bootstrap-simulation that includes both ageing error and growth variability</t>
-  </si>
-  <si>
     <t>Resample lengths for a given age after pooling age-length data across survey years ('Pooled') or using annual age-length data ('Annual')</t>
   </si>
   <si>
     <t>Implement 1 cm, 2 cm, and 5 cm length bins in the length data</t>
   </si>
   <si>
-    <t>Aggregate length and age data before  ('pre') or after ('post') length and age expansion</t>
+    <t>Standard bootstrap-simulation (ommiting steps 5 and 6 that include ageing error and growth variability in the Bootstrap-Simulation framework)</t>
+  </si>
+  <si>
+    <t>Bootstrap-simulation including both ageing error and growth variability</t>
+  </si>
+  <si>
+    <t>Aggregate length and age data before  ('Pre-expansion') or after ('Post-expansion') length and age expansion</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -101,7 +101,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -109,12 +109,54 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -398,86 +440,93 @@
   <dimension ref="B2:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B3" sqref="B3:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="81.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+      <c r="B2" s="1"/>
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" s="3"/>
+    </row>
+    <row r="4" spans="2:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+      <c r="C5" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C6" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="8"/>
+    </row>
+    <row r="9" spans="2:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B9" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s">
+    <row r="10" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
+    <row r="11" spans="2:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B11" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C11" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" t="s">
-        <v>17</v>
-      </c>
-    </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B8:C8"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>